<commit_message>
Exe 11 - collection
</commit_message>
<xml_diff>
--- a/me/1.Lap-trinh-python/5.su-dung-labrary.xlsx
+++ b/me/1.Lap-trinh-python/5.su-dung-labrary.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vudinhquang/Documents/quang/python/me/1.Lap-trinh-python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A2BCF8-9C80-D341-B01B-404059F07DA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F2734AB-4194-5840-B475-EC5BE4CDB7EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{0C205979-F84C-2240-84A8-CC7BE85DA138}"/>
+    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{0C205979-F84C-2240-84A8-CC7BE85DA138}"/>
   </bookViews>
   <sheets>
     <sheet name="Lib 01" sheetId="1" r:id="rId1"/>
     <sheet name="Lib 02" sheetId="2" r:id="rId2"/>
+    <sheet name="Exe 11 - collection" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="114">
   <si>
     <t>構成</t>
   </si>
@@ -408,6 +409,36 @@
   </si>
   <si>
     <t>import showInfo và returnInfo từ mlib</t>
+  </si>
+  <si>
+    <t>exe_11_collection.py</t>
+  </si>
+  <si>
+    <t>Merge two dictionaries and Sum the Values</t>
+  </si>
+  <si>
+    <t>python/exe/exe_11_collection.py</t>
+  </si>
+  <si>
+    <t>from collections import Counter</t>
+  </si>
+  <si>
+    <t>dictOne = {'a': 100, 'b': 100, 'c':300}</t>
+  </si>
+  <si>
+    <t>dictTwo = {'a': 300, 'b': 200, 'd':400, 'c':400}</t>
+  </si>
+  <si>
+    <t>result  = dict(Counter(dictOne)+Counter(dictTwo))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">print(result) </t>
+  </si>
+  <si>
+    <t>python3 exe_11_collection.py</t>
+  </si>
+  <si>
+    <t>Run</t>
   </si>
 </sst>
 </file>
@@ -562,9 +593,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1265,6 +1296,426 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>101599</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>495002</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5AF42E51-F41B-E252-E58F-0F5DD8E85F95}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="927099" y="12903200"/>
+          <a:ext cx="10299403" cy="965200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89EB468D-A98B-7285-9FC3-AE6B125525AF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1828800" y="10731500"/>
+          <a:ext cx="0" cy="139700"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>711200</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE96A8ED-8BC5-D647-C9D6-37FDC6E3F797}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1536700" y="10960100"/>
+          <a:ext cx="292100" cy="2527300"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>711200</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D86F63B3-8C63-5E0C-D035-FD732F565E80}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2362200" y="10756900"/>
+          <a:ext cx="12700" cy="101600"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D358772-B898-B7A9-3620-1058945A6B30}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2374900" y="10947400"/>
+          <a:ext cx="0" cy="2527300"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Straight Arrow Connector 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC73C36F-B3D7-40DA-0614-22930B6ABB5A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3009900" y="10731500"/>
+          <a:ext cx="393700" cy="101600"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Straight Arrow Connector 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E86769D4-0322-C5B3-3EAE-9A296159F378}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="3263900" y="10947400"/>
+          <a:ext cx="165100" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Straight Arrow Connector 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3CBEF196-DA6C-1DB7-7EED-FC77FB577F80}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2908300" y="10947400"/>
+          <a:ext cx="1181100" cy="2552700"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2676,8 +3127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46DF4545-DF05-FF46-B8AF-DE4FE48D251A}">
   <dimension ref="A2:P135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="F145" sqref="F145"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="M47" sqref="M47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2859,21 +3310,21 @@
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B29" s="4"/>
-      <c r="D29" s="13" t="s">
+      <c r="D29" t="s">
         <v>38</v>
       </c>
       <c r="F29" s="5"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B30" s="4"/>
-      <c r="D30" s="13" t="s">
+      <c r="D30" t="s">
         <v>67</v>
       </c>
       <c r="F30" s="5"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B31" s="4"/>
-      <c r="D31" s="13" t="s">
+      <c r="D31" t="s">
         <v>68</v>
       </c>
       <c r="F31" s="5"/>
@@ -3011,30 +3462,22 @@
       <c r="B51" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C51" s="14"/>
-      <c r="D51" s="14"/>
       <c r="E51" s="5"/>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B52" s="4"/>
-      <c r="C52" s="14"/>
-      <c r="D52" s="14"/>
       <c r="E52" s="5"/>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B53" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C53" s="14"/>
-      <c r="D53" s="14"/>
       <c r="E53" s="5"/>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B54" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C54" s="14"/>
-      <c r="D54" s="14"/>
       <c r="E54" s="5"/>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.2">
@@ -3044,7 +3487,7 @@
       <c r="E55" s="10"/>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A58" s="15" t="s">
+      <c r="A58" s="13" t="s">
         <v>78</v>
       </c>
     </row>
@@ -3075,17 +3518,6 @@
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="3"/>
-      <c r="E60" s="14"/>
-      <c r="F60" s="14"/>
-      <c r="G60" s="14"/>
-      <c r="H60" s="14"/>
-      <c r="I60" s="14"/>
-      <c r="J60" s="14"/>
-      <c r="K60" s="14"/>
-      <c r="L60" s="14"/>
-      <c r="M60" s="14"/>
-      <c r="N60" s="14"/>
-      <c r="O60" s="14"/>
       <c r="P60" s="5"/>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.2">
@@ -3093,23 +3525,13 @@
       <c r="B61" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C61" s="14"/>
       <c r="D61" s="5"/>
-      <c r="E61" s="14" t="s">
+      <c r="E61" t="s">
         <v>35</v>
       </c>
-      <c r="F61" s="14" t="s">
+      <c r="F61" t="s">
         <v>86</v>
       </c>
-      <c r="G61" s="14"/>
-      <c r="H61" s="14"/>
-      <c r="I61" s="14"/>
-      <c r="J61" s="14"/>
-      <c r="K61" s="14"/>
-      <c r="L61" s="14"/>
-      <c r="M61" s="14"/>
-      <c r="N61" s="14"/>
-      <c r="O61" s="14"/>
       <c r="P61" s="5"/>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.2">
@@ -3117,19 +3539,7 @@
       <c r="B62" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C62" s="14"/>
       <c r="D62" s="5"/>
-      <c r="E62" s="14"/>
-      <c r="F62" s="14"/>
-      <c r="G62" s="14"/>
-      <c r="H62" s="14"/>
-      <c r="I62" s="14"/>
-      <c r="J62" s="14"/>
-      <c r="K62" s="14"/>
-      <c r="L62" s="14"/>
-      <c r="M62" s="14"/>
-      <c r="N62" s="14"/>
-      <c r="O62" s="14"/>
       <c r="P62" s="5"/>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.2">
@@ -3137,19 +3547,7 @@
       <c r="B63" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C63" s="14"/>
       <c r="D63" s="5"/>
-      <c r="E63" s="14"/>
-      <c r="F63" s="14"/>
-      <c r="G63" s="14"/>
-      <c r="H63" s="14"/>
-      <c r="I63" s="14"/>
-      <c r="J63" s="14"/>
-      <c r="K63" s="14"/>
-      <c r="L63" s="14"/>
-      <c r="M63" s="14"/>
-      <c r="N63" s="14"/>
-      <c r="O63" s="14"/>
       <c r="P63" s="5"/>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.2">
@@ -3157,19 +3555,7 @@
       <c r="B64" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C64" s="14"/>
       <c r="D64" s="5"/>
-      <c r="E64" s="14"/>
-      <c r="F64" s="14"/>
-      <c r="G64" s="14"/>
-      <c r="H64" s="14"/>
-      <c r="I64" s="14"/>
-      <c r="J64" s="14"/>
-      <c r="K64" s="14"/>
-      <c r="L64" s="14"/>
-      <c r="M64" s="14"/>
-      <c r="N64" s="14"/>
-      <c r="O64" s="14"/>
       <c r="P64" s="5"/>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.2">
@@ -3177,35 +3563,10 @@
       <c r="B65" s="8"/>
       <c r="C65" s="9"/>
       <c r="D65" s="10"/>
-      <c r="E65" s="14"/>
-      <c r="F65" s="14"/>
-      <c r="G65" s="14"/>
-      <c r="H65" s="14"/>
-      <c r="I65" s="14"/>
-      <c r="J65" s="14"/>
-      <c r="K65" s="14"/>
-      <c r="L65" s="14"/>
-      <c r="M65" s="14"/>
-      <c r="N65" s="14"/>
-      <c r="O65" s="14"/>
       <c r="P65" s="5"/>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A66" s="4"/>
-      <c r="B66" s="14"/>
-      <c r="C66" s="14"/>
-      <c r="D66" s="14"/>
-      <c r="E66" s="14"/>
-      <c r="F66" s="14"/>
-      <c r="G66" s="14"/>
-      <c r="H66" s="14"/>
-      <c r="I66" s="14"/>
-      <c r="J66" s="14"/>
-      <c r="K66" s="14"/>
-      <c r="L66" s="14"/>
-      <c r="M66" s="14"/>
-      <c r="N66" s="14"/>
-      <c r="O66" s="14"/>
       <c r="P66" s="5"/>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.2">
@@ -3231,108 +3592,36 @@
     <row r="68" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A68" s="4"/>
       <c r="B68" s="4"/>
-      <c r="C68" s="14"/>
-      <c r="D68" s="14"/>
-      <c r="E68" s="14"/>
-      <c r="F68" s="14"/>
-      <c r="G68" s="14"/>
-      <c r="H68" s="14"/>
-      <c r="I68" s="14"/>
-      <c r="J68" s="14"/>
-      <c r="K68" s="14"/>
-      <c r="L68" s="14"/>
-      <c r="M68" s="14"/>
-      <c r="N68" s="14"/>
       <c r="O68" s="5"/>
       <c r="P68" s="5"/>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A69" s="4"/>
       <c r="B69" s="4"/>
-      <c r="C69" s="14"/>
-      <c r="D69" s="14"/>
-      <c r="E69" s="14"/>
-      <c r="F69" s="14"/>
-      <c r="G69" s="14"/>
-      <c r="H69" s="14"/>
-      <c r="I69" s="14"/>
-      <c r="J69" s="14"/>
-      <c r="K69" s="14"/>
-      <c r="L69" s="14"/>
-      <c r="M69" s="14"/>
-      <c r="N69" s="14"/>
       <c r="O69" s="5"/>
       <c r="P69" s="5"/>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
-      <c r="C70" s="14"/>
-      <c r="D70" s="14"/>
-      <c r="E70" s="14"/>
-      <c r="F70" s="14"/>
-      <c r="G70" s="14"/>
-      <c r="H70" s="14"/>
-      <c r="I70" s="14"/>
-      <c r="J70" s="14"/>
-      <c r="K70" s="14"/>
-      <c r="L70" s="14"/>
-      <c r="M70" s="14"/>
-      <c r="N70" s="14"/>
       <c r="O70" s="5"/>
       <c r="P70" s="5"/>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
-      <c r="C71" s="14"/>
-      <c r="D71" s="14"/>
-      <c r="E71" s="14"/>
-      <c r="F71" s="14"/>
-      <c r="G71" s="14"/>
-      <c r="H71" s="14"/>
-      <c r="I71" s="14"/>
-      <c r="J71" s="14"/>
-      <c r="K71" s="14"/>
-      <c r="L71" s="14"/>
-      <c r="M71" s="14"/>
-      <c r="N71" s="14"/>
       <c r="O71" s="5"/>
       <c r="P71" s="5"/>
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A72" s="4"/>
       <c r="B72" s="4"/>
-      <c r="C72" s="14"/>
-      <c r="D72" s="14"/>
-      <c r="E72" s="14"/>
-      <c r="F72" s="14"/>
-      <c r="G72" s="14"/>
-      <c r="H72" s="14"/>
-      <c r="I72" s="14"/>
-      <c r="J72" s="14"/>
-      <c r="K72" s="14"/>
-      <c r="L72" s="14"/>
-      <c r="M72" s="14"/>
-      <c r="N72" s="14"/>
       <c r="O72" s="5"/>
       <c r="P72" s="5"/>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
-      <c r="C73" s="14"/>
-      <c r="D73" s="14"/>
-      <c r="E73" s="14"/>
-      <c r="F73" s="14"/>
-      <c r="G73" s="14"/>
-      <c r="H73" s="14"/>
-      <c r="I73" s="14"/>
-      <c r="J73" s="14"/>
-      <c r="K73" s="14"/>
-      <c r="L73" s="14"/>
-      <c r="M73" s="14"/>
-      <c r="N73" s="14"/>
       <c r="O73" s="5"/>
       <c r="P73" s="5"/>
     </row>
@@ -3399,17 +3688,6 @@
       </c>
       <c r="C79" s="2"/>
       <c r="D79" s="3"/>
-      <c r="E79" s="14"/>
-      <c r="F79" s="14"/>
-      <c r="G79" s="14"/>
-      <c r="H79" s="14"/>
-      <c r="I79" s="14"/>
-      <c r="J79" s="14"/>
-      <c r="K79" s="14"/>
-      <c r="L79" s="14"/>
-      <c r="M79" s="14"/>
-      <c r="N79" s="14"/>
-      <c r="O79" s="14"/>
       <c r="P79" s="5"/>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.2">
@@ -3417,23 +3695,13 @@
       <c r="B80" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C80" s="14"/>
       <c r="D80" s="5"/>
-      <c r="E80" s="14" t="s">
+      <c r="E80" t="s">
         <v>35</v>
       </c>
-      <c r="F80" s="14" t="s">
+      <c r="F80" t="s">
         <v>92</v>
       </c>
-      <c r="G80" s="14"/>
-      <c r="H80" s="14"/>
-      <c r="I80" s="14"/>
-      <c r="J80" s="14"/>
-      <c r="K80" s="14"/>
-      <c r="L80" s="14"/>
-      <c r="M80" s="14"/>
-      <c r="N80" s="14"/>
-      <c r="O80" s="14"/>
       <c r="P80" s="5"/>
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.2">
@@ -3441,19 +3709,7 @@
       <c r="B81" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C81" s="14"/>
       <c r="D81" s="5"/>
-      <c r="E81" s="14"/>
-      <c r="F81" s="14"/>
-      <c r="G81" s="14"/>
-      <c r="H81" s="14"/>
-      <c r="I81" s="14"/>
-      <c r="J81" s="14"/>
-      <c r="K81" s="14"/>
-      <c r="L81" s="14"/>
-      <c r="M81" s="14"/>
-      <c r="N81" s="14"/>
-      <c r="O81" s="14"/>
       <c r="P81" s="5"/>
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.2">
@@ -3461,19 +3717,7 @@
       <c r="B82" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C82" s="14"/>
       <c r="D82" s="5"/>
-      <c r="E82" s="14"/>
-      <c r="F82" s="14"/>
-      <c r="G82" s="14"/>
-      <c r="H82" s="14"/>
-      <c r="I82" s="14"/>
-      <c r="J82" s="14"/>
-      <c r="K82" s="14"/>
-      <c r="L82" s="14"/>
-      <c r="M82" s="14"/>
-      <c r="N82" s="14"/>
-      <c r="O82" s="14"/>
       <c r="P82" s="5"/>
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.2">
@@ -3481,19 +3725,7 @@
       <c r="B83" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C83" s="14"/>
       <c r="D83" s="5"/>
-      <c r="E83" s="14"/>
-      <c r="F83" s="14"/>
-      <c r="G83" s="14"/>
-      <c r="H83" s="14"/>
-      <c r="I83" s="14"/>
-      <c r="J83" s="14"/>
-      <c r="K83" s="14"/>
-      <c r="L83" s="14"/>
-      <c r="M83" s="14"/>
-      <c r="N83" s="14"/>
-      <c r="O83" s="14"/>
       <c r="P83" s="5"/>
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.2">
@@ -3501,53 +3733,14 @@
       <c r="B84" s="8"/>
       <c r="C84" s="9"/>
       <c r="D84" s="10"/>
-      <c r="E84" s="14"/>
-      <c r="F84" s="14"/>
-      <c r="G84" s="14"/>
-      <c r="H84" s="14"/>
-      <c r="I84" s="14"/>
-      <c r="J84" s="14"/>
-      <c r="K84" s="14"/>
-      <c r="L84" s="14"/>
-      <c r="M84" s="14"/>
-      <c r="N84" s="14"/>
-      <c r="O84" s="14"/>
       <c r="P84" s="5"/>
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A85" s="4"/>
-      <c r="B85" s="14"/>
-      <c r="C85" s="14"/>
-      <c r="D85" s="14"/>
-      <c r="E85" s="14"/>
-      <c r="F85" s="14"/>
-      <c r="G85" s="14"/>
-      <c r="H85" s="14"/>
-      <c r="I85" s="14"/>
-      <c r="J85" s="14"/>
-      <c r="K85" s="14"/>
-      <c r="L85" s="14"/>
-      <c r="M85" s="14"/>
-      <c r="N85" s="14"/>
-      <c r="O85" s="14"/>
       <c r="P85" s="5"/>
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A86" s="4"/>
-      <c r="B86" s="14"/>
-      <c r="C86" s="14"/>
-      <c r="D86" s="14"/>
-      <c r="E86" s="14"/>
-      <c r="F86" s="14"/>
-      <c r="G86" s="14"/>
-      <c r="H86" s="14"/>
-      <c r="I86" s="14"/>
-      <c r="J86" s="14"/>
-      <c r="K86" s="14"/>
-      <c r="L86" s="14"/>
-      <c r="M86" s="14"/>
-      <c r="N86" s="14"/>
-      <c r="O86" s="14"/>
       <c r="P86" s="5"/>
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.2">
@@ -3573,108 +3766,36 @@
     <row r="88" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A88" s="4"/>
       <c r="B88" s="4"/>
-      <c r="C88" s="14"/>
-      <c r="D88" s="14"/>
-      <c r="E88" s="14"/>
-      <c r="F88" s="14"/>
-      <c r="G88" s="14"/>
-      <c r="H88" s="14"/>
-      <c r="I88" s="14"/>
-      <c r="J88" s="14"/>
-      <c r="K88" s="14"/>
-      <c r="L88" s="14"/>
-      <c r="M88" s="14"/>
-      <c r="N88" s="14"/>
       <c r="O88" s="5"/>
       <c r="P88" s="5"/>
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A89" s="4"/>
       <c r="B89" s="4"/>
-      <c r="C89" s="14"/>
-      <c r="D89" s="14"/>
-      <c r="E89" s="14"/>
-      <c r="F89" s="14"/>
-      <c r="G89" s="14"/>
-      <c r="H89" s="14"/>
-      <c r="I89" s="14"/>
-      <c r="J89" s="14"/>
-      <c r="K89" s="14"/>
-      <c r="L89" s="14"/>
-      <c r="M89" s="14"/>
-      <c r="N89" s="14"/>
       <c r="O89" s="5"/>
       <c r="P89" s="5"/>
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A90" s="4"/>
       <c r="B90" s="4"/>
-      <c r="C90" s="14"/>
-      <c r="D90" s="14"/>
-      <c r="E90" s="14"/>
-      <c r="F90" s="14"/>
-      <c r="G90" s="14"/>
-      <c r="H90" s="14"/>
-      <c r="I90" s="14"/>
-      <c r="J90" s="14"/>
-      <c r="K90" s="14"/>
-      <c r="L90" s="14"/>
-      <c r="M90" s="14"/>
-      <c r="N90" s="14"/>
       <c r="O90" s="5"/>
       <c r="P90" s="5"/>
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A91" s="4"/>
       <c r="B91" s="4"/>
-      <c r="C91" s="14"/>
-      <c r="D91" s="14"/>
-      <c r="E91" s="14"/>
-      <c r="F91" s="14"/>
-      <c r="G91" s="14"/>
-      <c r="H91" s="14"/>
-      <c r="I91" s="14"/>
-      <c r="J91" s="14"/>
-      <c r="K91" s="14"/>
-      <c r="L91" s="14"/>
-      <c r="M91" s="14"/>
-      <c r="N91" s="14"/>
       <c r="O91" s="5"/>
       <c r="P91" s="5"/>
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A92" s="4"/>
       <c r="B92" s="4"/>
-      <c r="C92" s="14"/>
-      <c r="D92" s="14"/>
-      <c r="E92" s="14"/>
-      <c r="F92" s="14"/>
-      <c r="G92" s="14"/>
-      <c r="H92" s="14"/>
-      <c r="I92" s="14"/>
-      <c r="J92" s="14"/>
-      <c r="K92" s="14"/>
-      <c r="L92" s="14"/>
-      <c r="M92" s="14"/>
-      <c r="N92" s="14"/>
       <c r="O92" s="5"/>
       <c r="P92" s="5"/>
     </row>
     <row r="93" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A93" s="4"/>
       <c r="B93" s="4"/>
-      <c r="C93" s="14"/>
-      <c r="D93" s="14"/>
-      <c r="E93" s="14"/>
-      <c r="F93" s="14"/>
-      <c r="G93" s="14"/>
-      <c r="H93" s="14"/>
-      <c r="I93" s="14"/>
-      <c r="J93" s="14"/>
-      <c r="K93" s="14"/>
-      <c r="L93" s="14"/>
-      <c r="M93" s="14"/>
-      <c r="N93" s="14"/>
       <c r="O93" s="5"/>
       <c r="P93" s="5"/>
     </row>
@@ -3741,17 +3862,6 @@
       </c>
       <c r="C99" s="2"/>
       <c r="D99" s="3"/>
-      <c r="E99" s="14"/>
-      <c r="F99" s="14"/>
-      <c r="G99" s="14"/>
-      <c r="H99" s="14"/>
-      <c r="I99" s="14"/>
-      <c r="J99" s="14"/>
-      <c r="K99" s="14"/>
-      <c r="L99" s="14"/>
-      <c r="M99" s="14"/>
-      <c r="N99" s="14"/>
-      <c r="O99" s="14"/>
       <c r="P99" s="5"/>
     </row>
     <row r="100" spans="1:16" x14ac:dyDescent="0.2">
@@ -3759,23 +3869,13 @@
       <c r="B100" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C100" s="14"/>
       <c r="D100" s="5"/>
-      <c r="E100" s="14" t="s">
+      <c r="E100" t="s">
         <v>35</v>
       </c>
-      <c r="F100" s="14" t="s">
+      <c r="F100" t="s">
         <v>98</v>
       </c>
-      <c r="G100" s="14"/>
-      <c r="H100" s="14"/>
-      <c r="I100" s="14"/>
-      <c r="J100" s="14"/>
-      <c r="K100" s="14"/>
-      <c r="L100" s="14"/>
-      <c r="M100" s="14"/>
-      <c r="N100" s="14"/>
-      <c r="O100" s="14"/>
       <c r="P100" s="5"/>
     </row>
     <row r="101" spans="1:16" x14ac:dyDescent="0.2">
@@ -3783,23 +3883,13 @@
       <c r="B101" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C101" s="14"/>
       <c r="D101" s="5"/>
-      <c r="E101" s="14" t="s">
+      <c r="E101" t="s">
         <v>35</v>
       </c>
-      <c r="F101" s="14" t="s">
+      <c r="F101" t="s">
         <v>99</v>
       </c>
-      <c r="G101" s="14"/>
-      <c r="H101" s="14"/>
-      <c r="I101" s="14"/>
-      <c r="J101" s="14"/>
-      <c r="K101" s="14"/>
-      <c r="L101" s="14"/>
-      <c r="M101" s="14"/>
-      <c r="N101" s="14"/>
-      <c r="O101" s="14"/>
       <c r="P101" s="5"/>
     </row>
     <row r="102" spans="1:16" x14ac:dyDescent="0.2">
@@ -3807,19 +3897,7 @@
       <c r="B102" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C102" s="14"/>
       <c r="D102" s="5"/>
-      <c r="E102" s="14"/>
-      <c r="F102" s="14"/>
-      <c r="G102" s="14"/>
-      <c r="H102" s="14"/>
-      <c r="I102" s="14"/>
-      <c r="J102" s="14"/>
-      <c r="K102" s="14"/>
-      <c r="L102" s="14"/>
-      <c r="M102" s="14"/>
-      <c r="N102" s="14"/>
-      <c r="O102" s="14"/>
       <c r="P102" s="5"/>
     </row>
     <row r="103" spans="1:16" x14ac:dyDescent="0.2">
@@ -3827,19 +3905,7 @@
       <c r="B103" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C103" s="14"/>
       <c r="D103" s="5"/>
-      <c r="E103" s="14"/>
-      <c r="F103" s="14"/>
-      <c r="G103" s="14"/>
-      <c r="H103" s="14"/>
-      <c r="I103" s="14"/>
-      <c r="J103" s="14"/>
-      <c r="K103" s="14"/>
-      <c r="L103" s="14"/>
-      <c r="M103" s="14"/>
-      <c r="N103" s="14"/>
-      <c r="O103" s="14"/>
       <c r="P103" s="5"/>
     </row>
     <row r="104" spans="1:16" x14ac:dyDescent="0.2">
@@ -3847,53 +3913,14 @@
       <c r="B104" s="8"/>
       <c r="C104" s="9"/>
       <c r="D104" s="10"/>
-      <c r="E104" s="14"/>
-      <c r="F104" s="14"/>
-      <c r="G104" s="14"/>
-      <c r="H104" s="14"/>
-      <c r="I104" s="14"/>
-      <c r="J104" s="14"/>
-      <c r="K104" s="14"/>
-      <c r="L104" s="14"/>
-      <c r="M104" s="14"/>
-      <c r="N104" s="14"/>
-      <c r="O104" s="14"/>
       <c r="P104" s="5"/>
     </row>
     <row r="105" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A105" s="4"/>
-      <c r="B105" s="14"/>
-      <c r="C105" s="14"/>
-      <c r="D105" s="14"/>
-      <c r="E105" s="14"/>
-      <c r="F105" s="14"/>
-      <c r="G105" s="14"/>
-      <c r="H105" s="14"/>
-      <c r="I105" s="14"/>
-      <c r="J105" s="14"/>
-      <c r="K105" s="14"/>
-      <c r="L105" s="14"/>
-      <c r="M105" s="14"/>
-      <c r="N105" s="14"/>
-      <c r="O105" s="14"/>
       <c r="P105" s="5"/>
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A106" s="4"/>
-      <c r="B106" s="14"/>
-      <c r="C106" s="14"/>
-      <c r="D106" s="14"/>
-      <c r="E106" s="14"/>
-      <c r="F106" s="14"/>
-      <c r="G106" s="14"/>
-      <c r="H106" s="14"/>
-      <c r="I106" s="14"/>
-      <c r="J106" s="14"/>
-      <c r="K106" s="14"/>
-      <c r="L106" s="14"/>
-      <c r="M106" s="14"/>
-      <c r="N106" s="14"/>
-      <c r="O106" s="14"/>
       <c r="P106" s="5"/>
     </row>
     <row r="107" spans="1:16" x14ac:dyDescent="0.2">
@@ -3919,108 +3946,36 @@
     <row r="108" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A108" s="4"/>
       <c r="B108" s="4"/>
-      <c r="C108" s="14"/>
-      <c r="D108" s="14"/>
-      <c r="E108" s="14"/>
-      <c r="F108" s="14"/>
-      <c r="G108" s="14"/>
-      <c r="H108" s="14"/>
-      <c r="I108" s="14"/>
-      <c r="J108" s="14"/>
-      <c r="K108" s="14"/>
-      <c r="L108" s="14"/>
-      <c r="M108" s="14"/>
-      <c r="N108" s="14"/>
       <c r="O108" s="5"/>
       <c r="P108" s="5"/>
     </row>
     <row r="109" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A109" s="4"/>
       <c r="B109" s="4"/>
-      <c r="C109" s="14"/>
-      <c r="D109" s="14"/>
-      <c r="E109" s="14"/>
-      <c r="F109" s="14"/>
-      <c r="G109" s="14"/>
-      <c r="H109" s="14"/>
-      <c r="I109" s="14"/>
-      <c r="J109" s="14"/>
-      <c r="K109" s="14"/>
-      <c r="L109" s="14"/>
-      <c r="M109" s="14"/>
-      <c r="N109" s="14"/>
       <c r="O109" s="5"/>
       <c r="P109" s="5"/>
     </row>
     <row r="110" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A110" s="4"/>
       <c r="B110" s="4"/>
-      <c r="C110" s="14"/>
-      <c r="D110" s="14"/>
-      <c r="E110" s="14"/>
-      <c r="F110" s="14"/>
-      <c r="G110" s="14"/>
-      <c r="H110" s="14"/>
-      <c r="I110" s="14"/>
-      <c r="J110" s="14"/>
-      <c r="K110" s="14"/>
-      <c r="L110" s="14"/>
-      <c r="M110" s="14"/>
-      <c r="N110" s="14"/>
       <c r="O110" s="5"/>
       <c r="P110" s="5"/>
     </row>
     <row r="111" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A111" s="4"/>
       <c r="B111" s="4"/>
-      <c r="C111" s="14"/>
-      <c r="D111" s="14"/>
-      <c r="E111" s="14"/>
-      <c r="F111" s="14"/>
-      <c r="G111" s="14"/>
-      <c r="H111" s="14"/>
-      <c r="I111" s="14"/>
-      <c r="J111" s="14"/>
-      <c r="K111" s="14"/>
-      <c r="L111" s="14"/>
-      <c r="M111" s="14"/>
-      <c r="N111" s="14"/>
       <c r="O111" s="5"/>
       <c r="P111" s="5"/>
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A112" s="4"/>
       <c r="B112" s="4"/>
-      <c r="C112" s="14"/>
-      <c r="D112" s="14"/>
-      <c r="E112" s="14"/>
-      <c r="F112" s="14"/>
-      <c r="G112" s="14"/>
-      <c r="H112" s="14"/>
-      <c r="I112" s="14"/>
-      <c r="J112" s="14"/>
-      <c r="K112" s="14"/>
-      <c r="L112" s="14"/>
-      <c r="M112" s="14"/>
-      <c r="N112" s="14"/>
       <c r="O112" s="5"/>
       <c r="P112" s="5"/>
     </row>
     <row r="113" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A113" s="4"/>
       <c r="B113" s="4"/>
-      <c r="C113" s="14"/>
-      <c r="D113" s="14"/>
-      <c r="E113" s="14"/>
-      <c r="F113" s="14"/>
-      <c r="G113" s="14"/>
-      <c r="H113" s="14"/>
-      <c r="I113" s="14"/>
-      <c r="J113" s="14"/>
-      <c r="K113" s="14"/>
-      <c r="L113" s="14"/>
-      <c r="M113" s="14"/>
-      <c r="N113" s="14"/>
       <c r="O113" s="5"/>
       <c r="P113" s="5"/>
     </row>
@@ -4088,16 +4043,6 @@
       <c r="C119" s="2"/>
       <c r="D119" s="2"/>
       <c r="E119" s="3"/>
-      <c r="F119" s="14"/>
-      <c r="G119" s="14"/>
-      <c r="H119" s="14"/>
-      <c r="I119" s="14"/>
-      <c r="J119" s="14"/>
-      <c r="K119" s="14"/>
-      <c r="L119" s="14"/>
-      <c r="M119" s="14"/>
-      <c r="N119" s="14"/>
-      <c r="O119" s="14"/>
       <c r="P119" s="5"/>
     </row>
     <row r="120" spans="1:16" x14ac:dyDescent="0.2">
@@ -4105,23 +4050,13 @@
       <c r="B120" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C120" s="14"/>
-      <c r="D120" s="14"/>
       <c r="E120" s="5"/>
-      <c r="F120" s="14" t="s">
+      <c r="F120" t="s">
         <v>35</v>
       </c>
-      <c r="G120" s="14" t="s">
+      <c r="G120" t="s">
         <v>103</v>
       </c>
-      <c r="H120" s="14"/>
-      <c r="I120" s="14"/>
-      <c r="J120" s="14"/>
-      <c r="K120" s="14"/>
-      <c r="L120" s="14"/>
-      <c r="M120" s="14"/>
-      <c r="N120" s="14"/>
-      <c r="O120" s="14"/>
       <c r="P120" s="5"/>
     </row>
     <row r="121" spans="1:16" x14ac:dyDescent="0.2">
@@ -4129,19 +4064,7 @@
       <c r="B121" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C121" s="14"/>
-      <c r="D121" s="14"/>
       <c r="E121" s="5"/>
-      <c r="F121" s="14"/>
-      <c r="G121" s="14"/>
-      <c r="H121" s="14"/>
-      <c r="I121" s="14"/>
-      <c r="J121" s="14"/>
-      <c r="K121" s="14"/>
-      <c r="L121" s="14"/>
-      <c r="M121" s="14"/>
-      <c r="N121" s="14"/>
-      <c r="O121" s="14"/>
       <c r="P121" s="5"/>
     </row>
     <row r="122" spans="1:16" x14ac:dyDescent="0.2">
@@ -4149,19 +4072,7 @@
       <c r="B122" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C122" s="14"/>
-      <c r="D122" s="14"/>
       <c r="E122" s="5"/>
-      <c r="F122" s="14"/>
-      <c r="G122" s="14"/>
-      <c r="H122" s="14"/>
-      <c r="I122" s="14"/>
-      <c r="J122" s="14"/>
-      <c r="K122" s="14"/>
-      <c r="L122" s="14"/>
-      <c r="M122" s="14"/>
-      <c r="N122" s="14"/>
-      <c r="O122" s="14"/>
       <c r="P122" s="5"/>
     </row>
     <row r="123" spans="1:16" x14ac:dyDescent="0.2">
@@ -4169,19 +4080,7 @@
       <c r="B123" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C123" s="14"/>
-      <c r="D123" s="14"/>
       <c r="E123" s="5"/>
-      <c r="F123" s="14"/>
-      <c r="G123" s="14"/>
-      <c r="H123" s="14"/>
-      <c r="I123" s="14"/>
-      <c r="J123" s="14"/>
-      <c r="K123" s="14"/>
-      <c r="L123" s="14"/>
-      <c r="M123" s="14"/>
-      <c r="N123" s="14"/>
-      <c r="O123" s="14"/>
       <c r="P123" s="5"/>
     </row>
     <row r="124" spans="1:16" x14ac:dyDescent="0.2">
@@ -4190,52 +4089,14 @@
       <c r="C124" s="9"/>
       <c r="D124" s="9"/>
       <c r="E124" s="10"/>
-      <c r="F124" s="14"/>
-      <c r="G124" s="14"/>
-      <c r="H124" s="14"/>
-      <c r="I124" s="14"/>
-      <c r="J124" s="14"/>
-      <c r="K124" s="14"/>
-      <c r="L124" s="14"/>
-      <c r="M124" s="14"/>
-      <c r="N124" s="14"/>
-      <c r="O124" s="14"/>
       <c r="P124" s="5"/>
     </row>
     <row r="125" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A125" s="4"/>
-      <c r="B125" s="14"/>
-      <c r="C125" s="14"/>
-      <c r="D125" s="14"/>
-      <c r="E125" s="14"/>
-      <c r="F125" s="14"/>
-      <c r="G125" s="14"/>
-      <c r="H125" s="14"/>
-      <c r="I125" s="14"/>
-      <c r="J125" s="14"/>
-      <c r="K125" s="14"/>
-      <c r="L125" s="14"/>
-      <c r="M125" s="14"/>
-      <c r="N125" s="14"/>
-      <c r="O125" s="14"/>
       <c r="P125" s="5"/>
     </row>
     <row r="126" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A126" s="4"/>
-      <c r="B126" s="14"/>
-      <c r="C126" s="14"/>
-      <c r="D126" s="14"/>
-      <c r="E126" s="14"/>
-      <c r="F126" s="14"/>
-      <c r="G126" s="14"/>
-      <c r="H126" s="14"/>
-      <c r="I126" s="14"/>
-      <c r="J126" s="14"/>
-      <c r="K126" s="14"/>
-      <c r="L126" s="14"/>
-      <c r="M126" s="14"/>
-      <c r="N126" s="14"/>
-      <c r="O126" s="14"/>
       <c r="P126" s="5"/>
     </row>
     <row r="127" spans="1:16" x14ac:dyDescent="0.2">
@@ -4261,108 +4122,36 @@
     <row r="128" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A128" s="4"/>
       <c r="B128" s="4"/>
-      <c r="C128" s="14"/>
-      <c r="D128" s="14"/>
-      <c r="E128" s="14"/>
-      <c r="F128" s="14"/>
-      <c r="G128" s="14"/>
-      <c r="H128" s="14"/>
-      <c r="I128" s="14"/>
-      <c r="J128" s="14"/>
-      <c r="K128" s="14"/>
-      <c r="L128" s="14"/>
-      <c r="M128" s="14"/>
-      <c r="N128" s="14"/>
       <c r="O128" s="5"/>
       <c r="P128" s="5"/>
     </row>
     <row r="129" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A129" s="4"/>
       <c r="B129" s="4"/>
-      <c r="C129" s="14"/>
-      <c r="D129" s="14"/>
-      <c r="E129" s="14"/>
-      <c r="F129" s="14"/>
-      <c r="G129" s="14"/>
-      <c r="H129" s="14"/>
-      <c r="I129" s="14"/>
-      <c r="J129" s="14"/>
-      <c r="K129" s="14"/>
-      <c r="L129" s="14"/>
-      <c r="M129" s="14"/>
-      <c r="N129" s="14"/>
       <c r="O129" s="5"/>
       <c r="P129" s="5"/>
     </row>
     <row r="130" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A130" s="4"/>
       <c r="B130" s="4"/>
-      <c r="C130" s="14"/>
-      <c r="D130" s="14"/>
-      <c r="E130" s="14"/>
-      <c r="F130" s="14"/>
-      <c r="G130" s="14"/>
-      <c r="H130" s="14"/>
-      <c r="I130" s="14"/>
-      <c r="J130" s="14"/>
-      <c r="K130" s="14"/>
-      <c r="L130" s="14"/>
-      <c r="M130" s="14"/>
-      <c r="N130" s="14"/>
       <c r="O130" s="5"/>
       <c r="P130" s="5"/>
     </row>
     <row r="131" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A131" s="4"/>
       <c r="B131" s="4"/>
-      <c r="C131" s="14"/>
-      <c r="D131" s="14"/>
-      <c r="E131" s="14"/>
-      <c r="F131" s="14"/>
-      <c r="G131" s="14"/>
-      <c r="H131" s="14"/>
-      <c r="I131" s="14"/>
-      <c r="J131" s="14"/>
-      <c r="K131" s="14"/>
-      <c r="L131" s="14"/>
-      <c r="M131" s="14"/>
-      <c r="N131" s="14"/>
       <c r="O131" s="5"/>
       <c r="P131" s="5"/>
     </row>
     <row r="132" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A132" s="4"/>
       <c r="B132" s="4"/>
-      <c r="C132" s="14"/>
-      <c r="D132" s="14"/>
-      <c r="E132" s="14"/>
-      <c r="F132" s="14"/>
-      <c r="G132" s="14"/>
-      <c r="H132" s="14"/>
-      <c r="I132" s="14"/>
-      <c r="J132" s="14"/>
-      <c r="K132" s="14"/>
-      <c r="L132" s="14"/>
-      <c r="M132" s="14"/>
-      <c r="N132" s="14"/>
       <c r="O132" s="5"/>
       <c r="P132" s="5"/>
     </row>
     <row r="133" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A133" s="4"/>
       <c r="B133" s="4"/>
-      <c r="C133" s="14"/>
-      <c r="D133" s="14"/>
-      <c r="E133" s="14"/>
-      <c r="F133" s="14"/>
-      <c r="G133" s="14"/>
-      <c r="H133" s="14"/>
-      <c r="I133" s="14"/>
-      <c r="J133" s="14"/>
-      <c r="K133" s="14"/>
-      <c r="L133" s="14"/>
-      <c r="M133" s="14"/>
-      <c r="N133" s="14"/>
       <c r="O133" s="5"/>
       <c r="P133" s="5"/>
     </row>
@@ -4406,4 +4195,543 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AAE6958-7DBB-C54C-B5F4-6EED720F6C8F}">
+  <dimension ref="A2:N69"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="I55" sqref="I55"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B7" s="4"/>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B8" s="4"/>
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="4"/>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B10" s="4"/>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B11" s="4"/>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B12" s="4"/>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B13" s="4"/>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B14" s="4"/>
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B15" s="4"/>
+      <c r="D15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B16" s="4"/>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B17" s="4"/>
+      <c r="D17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B18" s="4"/>
+      <c r="D18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="5"/>
+      <c r="H18" s="6"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B19" s="4"/>
+      <c r="D19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B20" s="4"/>
+      <c r="C20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="7"/>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B21" s="4"/>
+      <c r="D21" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B22" s="4"/>
+      <c r="D22" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B23" s="4"/>
+      <c r="D23" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B24" s="4"/>
+      <c r="D24" t="s">
+        <v>19</v>
+      </c>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B25" s="4"/>
+      <c r="C25" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B26" s="4"/>
+      <c r="D26" t="s">
+        <v>21</v>
+      </c>
+      <c r="F26" s="5"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B27" s="4"/>
+      <c r="D27" t="s">
+        <v>22</v>
+      </c>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B28" s="4"/>
+      <c r="C28" t="s">
+        <v>37</v>
+      </c>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B29" s="4"/>
+      <c r="D29" t="s">
+        <v>38</v>
+      </c>
+      <c r="F29" s="5"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B30" s="4"/>
+      <c r="D30" t="s">
+        <v>67</v>
+      </c>
+      <c r="F30" s="5"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B31" s="4"/>
+      <c r="D31" t="s">
+        <v>68</v>
+      </c>
+      <c r="F31" s="5"/>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B32" s="4"/>
+      <c r="D32" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="F32" s="5"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B33" s="4"/>
+      <c r="D33" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="F33" s="5"/>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B34" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F34" s="5"/>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B35" s="4"/>
+      <c r="C35" t="s">
+        <v>24</v>
+      </c>
+      <c r="F35" s="5"/>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B36" s="4"/>
+      <c r="C36" t="s">
+        <v>25</v>
+      </c>
+      <c r="F36" s="5"/>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B37" s="4"/>
+      <c r="C37" t="s">
+        <v>26</v>
+      </c>
+      <c r="F37" s="5"/>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B38" s="4"/>
+      <c r="C38" t="s">
+        <v>27</v>
+      </c>
+      <c r="F38" s="5"/>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B39" s="4"/>
+      <c r="C39" t="s">
+        <v>28</v>
+      </c>
+      <c r="F39" s="5"/>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B40" s="4"/>
+      <c r="C40" t="s">
+        <v>29</v>
+      </c>
+      <c r="F40" s="5"/>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B41" s="4"/>
+      <c r="C41" t="s">
+        <v>30</v>
+      </c>
+      <c r="F41" s="5"/>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B42" s="4"/>
+      <c r="C42" t="s">
+        <v>31</v>
+      </c>
+      <c r="F42" s="5"/>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B43" s="4"/>
+      <c r="C43" t="s">
+        <v>32</v>
+      </c>
+      <c r="F43" s="5"/>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B44" s="4"/>
+      <c r="C44" t="s">
+        <v>33</v>
+      </c>
+      <c r="F44" s="5"/>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B45" s="4"/>
+      <c r="C45" t="s">
+        <v>34</v>
+      </c>
+      <c r="F45" s="5"/>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B46" s="4"/>
+      <c r="C46" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="F46" s="5"/>
+      <c r="G46" t="s">
+        <v>35</v>
+      </c>
+      <c r="H46" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B47" s="8"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="10"/>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A50" s="13" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B51" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="3"/>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B52" s="4"/>
+      <c r="C52" s="15"/>
+      <c r="D52" s="15"/>
+      <c r="E52" s="15"/>
+      <c r="F52" s="5"/>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B53" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C53" s="15"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="15"/>
+      <c r="F53" s="5"/>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B54" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C54" s="15"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="15"/>
+      <c r="F54" s="5"/>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B55" s="4"/>
+      <c r="C55" s="15"/>
+      <c r="D55" s="15"/>
+      <c r="E55" s="15"/>
+      <c r="F55" s="5"/>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B56" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C56" s="15"/>
+      <c r="D56" s="15"/>
+      <c r="E56" s="15"/>
+      <c r="F56" s="5"/>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B57" s="4"/>
+      <c r="C57" s="15"/>
+      <c r="D57" s="15"/>
+      <c r="E57" s="15"/>
+      <c r="F57" s="5"/>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B58" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C58" s="15"/>
+      <c r="D58" s="15"/>
+      <c r="E58" s="15"/>
+      <c r="F58" s="5"/>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B59" s="8"/>
+      <c r="C59" s="9"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="9"/>
+      <c r="F59" s="10"/>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A62" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="B62" s="2"/>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2"/>
+      <c r="G62" s="2"/>
+      <c r="H62" s="2"/>
+      <c r="I62" s="2"/>
+      <c r="J62" s="2"/>
+      <c r="K62" s="2"/>
+      <c r="L62" s="2"/>
+      <c r="M62" s="2"/>
+      <c r="N62" s="3"/>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A63" s="4"/>
+      <c r="B63" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="C63" s="15"/>
+      <c r="D63" s="15"/>
+      <c r="E63" s="15"/>
+      <c r="F63" s="15"/>
+      <c r="G63" s="15"/>
+      <c r="H63" s="15"/>
+      <c r="I63" s="15"/>
+      <c r="J63" s="15"/>
+      <c r="K63" s="15"/>
+      <c r="L63" s="15"/>
+      <c r="M63" s="15"/>
+      <c r="N63" s="5"/>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A64" s="4"/>
+      <c r="B64" s="15"/>
+      <c r="C64" s="15"/>
+      <c r="D64" s="15"/>
+      <c r="E64" s="15"/>
+      <c r="F64" s="15"/>
+      <c r="G64" s="15"/>
+      <c r="H64" s="15"/>
+      <c r="I64" s="15"/>
+      <c r="J64" s="15"/>
+      <c r="K64" s="15"/>
+      <c r="L64" s="15"/>
+      <c r="M64" s="15"/>
+      <c r="N64" s="5"/>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A65" s="4"/>
+      <c r="B65" s="15"/>
+      <c r="C65" s="15"/>
+      <c r="D65" s="15"/>
+      <c r="E65" s="15"/>
+      <c r="F65" s="15"/>
+      <c r="G65" s="15"/>
+      <c r="H65" s="15"/>
+      <c r="I65" s="15"/>
+      <c r="J65" s="15"/>
+      <c r="K65" s="15"/>
+      <c r="L65" s="15"/>
+      <c r="M65" s="15"/>
+      <c r="N65" s="5"/>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A66" s="4"/>
+      <c r="B66" s="15"/>
+      <c r="C66" s="15"/>
+      <c r="D66" s="15"/>
+      <c r="E66" s="15"/>
+      <c r="F66" s="15"/>
+      <c r="G66" s="15"/>
+      <c r="H66" s="15"/>
+      <c r="I66" s="15"/>
+      <c r="J66" s="15"/>
+      <c r="K66" s="15"/>
+      <c r="L66" s="15"/>
+      <c r="M66" s="15"/>
+      <c r="N66" s="5"/>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A67" s="4"/>
+      <c r="B67" s="15"/>
+      <c r="C67" s="15"/>
+      <c r="D67" s="15"/>
+      <c r="E67" s="15"/>
+      <c r="F67" s="15"/>
+      <c r="G67" s="15"/>
+      <c r="H67" s="15"/>
+      <c r="I67" s="15"/>
+      <c r="J67" s="15"/>
+      <c r="K67" s="15"/>
+      <c r="L67" s="15"/>
+      <c r="M67" s="15"/>
+      <c r="N67" s="5"/>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A68" s="4"/>
+      <c r="B68" s="15"/>
+      <c r="C68" s="15"/>
+      <c r="D68" s="15"/>
+      <c r="E68" s="15"/>
+      <c r="F68" s="15"/>
+      <c r="G68" s="15"/>
+      <c r="H68" s="15"/>
+      <c r="I68" s="15"/>
+      <c r="J68" s="15"/>
+      <c r="K68" s="15"/>
+      <c r="L68" s="15"/>
+      <c r="M68" s="15"/>
+      <c r="N68" s="5"/>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A69" s="8"/>
+      <c r="B69" s="9"/>
+      <c r="C69" s="9"/>
+      <c r="D69" s="9"/>
+      <c r="E69" s="9"/>
+      <c r="F69" s="9"/>
+      <c r="G69" s="9"/>
+      <c r="H69" s="9"/>
+      <c r="I69" s="9"/>
+      <c r="J69" s="9"/>
+      <c r="K69" s="9"/>
+      <c r="L69" s="9"/>
+      <c r="M69" s="9"/>
+      <c r="N69" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Exe 12 - random
</commit_message>
<xml_diff>
--- a/me/1.Lap-trinh-python/5.su-dung-labrary.xlsx
+++ b/me/1.Lap-trinh-python/5.su-dung-labrary.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vudinhquang/Documents/quang/python/me/1.Lap-trinh-python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F2734AB-4194-5840-B475-EC5BE4CDB7EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F3BAAE-38FF-7F48-93EE-44F47EFADC3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{0C205979-F84C-2240-84A8-CC7BE85DA138}"/>
+    <workbookView xWindow="3900" yWindow="2180" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{0C205979-F84C-2240-84A8-CC7BE85DA138}"/>
   </bookViews>
   <sheets>
     <sheet name="Lib 01" sheetId="1" r:id="rId1"/>
     <sheet name="Lib 02" sheetId="2" r:id="rId2"/>
     <sheet name="Exe 11 - collection" sheetId="3" r:id="rId3"/>
+    <sheet name="Exe 12 - random" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="121">
   <si>
     <t>構成</t>
   </si>
@@ -439,6 +440,27 @@
   </si>
   <si>
     <t>Run</t>
+  </si>
+  <si>
+    <t>Get random 2 elements from List</t>
+  </si>
+  <si>
+    <t>exe_12_random.py</t>
+  </si>
+  <si>
+    <t>python/exe/exe_12_random.py</t>
+  </si>
+  <si>
+    <t>import random</t>
+  </si>
+  <si>
+    <t>myList = ['Red', 'Blue', 'Green', 'White', 'Black']</t>
+  </si>
+  <si>
+    <t>print(random.sample(myList, 2))</t>
+  </si>
+  <si>
+    <t>python3 exe_12_random.py</t>
   </si>
 </sst>
 </file>
@@ -1716,6 +1738,55 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>101599</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>347094</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E1C0E46-213A-79E8-8C42-B01A5F7DC8BE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="927099" y="12471400"/>
+          <a:ext cx="10976995" cy="1028700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -4201,8 +4272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AAE6958-7DBB-C54C-B5F4-6EED720F6C8F}">
   <dimension ref="A2:N69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="I55" sqref="I55"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4405,14 +4476,14 @@
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B32" s="4"/>
-      <c r="D32" s="14" t="s">
+      <c r="D32" t="s">
         <v>70</v>
       </c>
       <c r="F32" s="5"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B33" s="4"/>
-      <c r="D33" s="14" t="s">
+      <c r="D33" t="s">
         <v>71</v>
       </c>
       <c r="F33" s="5"/>
@@ -4536,59 +4607,38 @@
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B52" s="4"/>
-      <c r="C52" s="15"/>
-      <c r="D52" s="15"/>
-      <c r="E52" s="15"/>
       <c r="F52" s="5"/>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B53" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C53" s="15"/>
-      <c r="D53" s="15"/>
-      <c r="E53" s="15"/>
       <c r="F53" s="5"/>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B54" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="C54" s="15"/>
-      <c r="D54" s="15"/>
-      <c r="E54" s="15"/>
       <c r="F54" s="5"/>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B55" s="4"/>
-      <c r="C55" s="15"/>
-      <c r="D55" s="15"/>
-      <c r="E55" s="15"/>
       <c r="F55" s="5"/>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B56" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="C56" s="15"/>
-      <c r="D56" s="15"/>
-      <c r="E56" s="15"/>
       <c r="F56" s="5"/>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B57" s="4"/>
-      <c r="C57" s="15"/>
-      <c r="D57" s="15"/>
-      <c r="E57" s="15"/>
       <c r="F57" s="5"/>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B58" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C58" s="15"/>
-      <c r="D58" s="15"/>
-      <c r="E58" s="15"/>
       <c r="F58" s="5"/>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.2">
@@ -4618,100 +4668,29 @@
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" s="4"/>
-      <c r="B63" s="15" t="s">
+      <c r="B63" t="s">
         <v>112</v>
       </c>
-      <c r="C63" s="15"/>
-      <c r="D63" s="15"/>
-      <c r="E63" s="15"/>
-      <c r="F63" s="15"/>
-      <c r="G63" s="15"/>
-      <c r="H63" s="15"/>
-      <c r="I63" s="15"/>
-      <c r="J63" s="15"/>
-      <c r="K63" s="15"/>
-      <c r="L63" s="15"/>
-      <c r="M63" s="15"/>
       <c r="N63" s="5"/>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" s="4"/>
-      <c r="B64" s="15"/>
-      <c r="C64" s="15"/>
-      <c r="D64" s="15"/>
-      <c r="E64" s="15"/>
-      <c r="F64" s="15"/>
-      <c r="G64" s="15"/>
-      <c r="H64" s="15"/>
-      <c r="I64" s="15"/>
-      <c r="J64" s="15"/>
-      <c r="K64" s="15"/>
-      <c r="L64" s="15"/>
-      <c r="M64" s="15"/>
       <c r="N64" s="5"/>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" s="4"/>
-      <c r="B65" s="15"/>
-      <c r="C65" s="15"/>
-      <c r="D65" s="15"/>
-      <c r="E65" s="15"/>
-      <c r="F65" s="15"/>
-      <c r="G65" s="15"/>
-      <c r="H65" s="15"/>
-      <c r="I65" s="15"/>
-      <c r="J65" s="15"/>
-      <c r="K65" s="15"/>
-      <c r="L65" s="15"/>
-      <c r="M65" s="15"/>
       <c r="N65" s="5"/>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" s="4"/>
-      <c r="B66" s="15"/>
-      <c r="C66" s="15"/>
-      <c r="D66" s="15"/>
-      <c r="E66" s="15"/>
-      <c r="F66" s="15"/>
-      <c r="G66" s="15"/>
-      <c r="H66" s="15"/>
-      <c r="I66" s="15"/>
-      <c r="J66" s="15"/>
-      <c r="K66" s="15"/>
-      <c r="L66" s="15"/>
-      <c r="M66" s="15"/>
       <c r="N66" s="5"/>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" s="4"/>
-      <c r="B67" s="15"/>
-      <c r="C67" s="15"/>
-      <c r="D67" s="15"/>
-      <c r="E67" s="15"/>
-      <c r="F67" s="15"/>
-      <c r="G67" s="15"/>
-      <c r="H67" s="15"/>
-      <c r="I67" s="15"/>
-      <c r="J67" s="15"/>
-      <c r="K67" s="15"/>
-      <c r="L67" s="15"/>
-      <c r="M67" s="15"/>
       <c r="N67" s="5"/>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68" s="4"/>
-      <c r="B68" s="15"/>
-      <c r="C68" s="15"/>
-      <c r="D68" s="15"/>
-      <c r="E68" s="15"/>
-      <c r="F68" s="15"/>
-      <c r="G68" s="15"/>
-      <c r="H68" s="15"/>
-      <c r="I68" s="15"/>
-      <c r="J68" s="15"/>
-      <c r="K68" s="15"/>
-      <c r="L68" s="15"/>
-      <c r="M68" s="15"/>
       <c r="N68" s="5"/>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.2">
@@ -4734,4 +4713,533 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{628D80A5-F3DA-8842-97EA-8A3AC84D0C3D}">
+  <dimension ref="A2:O67"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="D75" sqref="D75"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B7" s="4"/>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B8" s="4"/>
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="4"/>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B10" s="4"/>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B11" s="4"/>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B12" s="4"/>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B13" s="4"/>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B14" s="4"/>
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B15" s="4"/>
+      <c r="D15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B16" s="4"/>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B17" s="4"/>
+      <c r="D17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B18" s="4"/>
+      <c r="D18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="5"/>
+      <c r="H18" s="6"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B19" s="4"/>
+      <c r="D19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B20" s="4"/>
+      <c r="C20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="7"/>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B21" s="4"/>
+      <c r="D21" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B22" s="4"/>
+      <c r="D22" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B23" s="4"/>
+      <c r="D23" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B24" s="4"/>
+      <c r="D24" t="s">
+        <v>19</v>
+      </c>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B25" s="4"/>
+      <c r="C25" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B26" s="4"/>
+      <c r="D26" t="s">
+        <v>21</v>
+      </c>
+      <c r="F26" s="5"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B27" s="4"/>
+      <c r="D27" t="s">
+        <v>22</v>
+      </c>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B28" s="4"/>
+      <c r="C28" t="s">
+        <v>37</v>
+      </c>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B29" s="4"/>
+      <c r="D29" t="s">
+        <v>38</v>
+      </c>
+      <c r="F29" s="5"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B30" s="4"/>
+      <c r="D30" t="s">
+        <v>67</v>
+      </c>
+      <c r="F30" s="5"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B31" s="4"/>
+      <c r="D31" t="s">
+        <v>68</v>
+      </c>
+      <c r="F31" s="5"/>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B32" s="4"/>
+      <c r="D32" t="s">
+        <v>70</v>
+      </c>
+      <c r="F32" s="5"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B33" s="4"/>
+      <c r="D33" t="s">
+        <v>71</v>
+      </c>
+      <c r="F33" s="5"/>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B34" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F34" s="5"/>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B35" s="4"/>
+      <c r="C35" t="s">
+        <v>24</v>
+      </c>
+      <c r="F35" s="5"/>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B36" s="4"/>
+      <c r="C36" t="s">
+        <v>25</v>
+      </c>
+      <c r="F36" s="5"/>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B37" s="4"/>
+      <c r="C37" t="s">
+        <v>26</v>
+      </c>
+      <c r="F37" s="5"/>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B38" s="4"/>
+      <c r="C38" t="s">
+        <v>27</v>
+      </c>
+      <c r="F38" s="5"/>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B39" s="4"/>
+      <c r="C39" t="s">
+        <v>28</v>
+      </c>
+      <c r="F39" s="5"/>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B40" s="4"/>
+      <c r="C40" t="s">
+        <v>29</v>
+      </c>
+      <c r="F40" s="5"/>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B41" s="4"/>
+      <c r="C41" t="s">
+        <v>30</v>
+      </c>
+      <c r="F41" s="5"/>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B42" s="4"/>
+      <c r="C42" t="s">
+        <v>31</v>
+      </c>
+      <c r="F42" s="5"/>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B43" s="4"/>
+      <c r="C43" t="s">
+        <v>32</v>
+      </c>
+      <c r="F43" s="5"/>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B44" s="4"/>
+      <c r="C44" t="s">
+        <v>33</v>
+      </c>
+      <c r="F44" s="5"/>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B45" s="4"/>
+      <c r="C45" t="s">
+        <v>34</v>
+      </c>
+      <c r="F45" s="5"/>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B46" s="4"/>
+      <c r="C46" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="F46" s="5"/>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B47" s="4"/>
+      <c r="C47" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="F47" s="5"/>
+      <c r="G47" t="s">
+        <v>35</v>
+      </c>
+      <c r="H47" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B48" s="8"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="10"/>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A51" s="13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B52" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="3"/>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B53" s="4"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="15"/>
+      <c r="F53" s="5"/>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B54" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C54" s="15"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="15"/>
+      <c r="F54" s="5"/>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B55" s="4"/>
+      <c r="C55" s="15"/>
+      <c r="D55" s="15"/>
+      <c r="E55" s="15"/>
+      <c r="F55" s="5"/>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B56" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C56" s="15"/>
+      <c r="D56" s="15"/>
+      <c r="E56" s="15"/>
+      <c r="F56" s="5"/>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B57" s="8"/>
+      <c r="C57" s="9"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="10"/>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A60" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="B60" s="2"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
+      <c r="F60" s="2"/>
+      <c r="G60" s="2"/>
+      <c r="H60" s="2"/>
+      <c r="I60" s="2"/>
+      <c r="J60" s="2"/>
+      <c r="K60" s="2"/>
+      <c r="L60" s="2"/>
+      <c r="M60" s="2"/>
+      <c r="N60" s="2"/>
+      <c r="O60" s="3"/>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A61" s="4"/>
+      <c r="B61" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="C61" s="15"/>
+      <c r="D61" s="15"/>
+      <c r="E61" s="15"/>
+      <c r="F61" s="15"/>
+      <c r="G61" s="15"/>
+      <c r="H61" s="15"/>
+      <c r="I61" s="15"/>
+      <c r="J61" s="15"/>
+      <c r="K61" s="15"/>
+      <c r="L61" s="15"/>
+      <c r="M61" s="15"/>
+      <c r="N61" s="15"/>
+      <c r="O61" s="5"/>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A62" s="4"/>
+      <c r="B62" s="15"/>
+      <c r="C62" s="15"/>
+      <c r="D62" s="15"/>
+      <c r="E62" s="15"/>
+      <c r="F62" s="15"/>
+      <c r="G62" s="15"/>
+      <c r="H62" s="15"/>
+      <c r="I62" s="15"/>
+      <c r="J62" s="15"/>
+      <c r="K62" s="15"/>
+      <c r="L62" s="15"/>
+      <c r="M62" s="15"/>
+      <c r="N62" s="15"/>
+      <c r="O62" s="5"/>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A63" s="4"/>
+      <c r="B63" s="15"/>
+      <c r="C63" s="15"/>
+      <c r="D63" s="15"/>
+      <c r="E63" s="15"/>
+      <c r="F63" s="15"/>
+      <c r="G63" s="15"/>
+      <c r="H63" s="15"/>
+      <c r="I63" s="15"/>
+      <c r="J63" s="15"/>
+      <c r="K63" s="15"/>
+      <c r="L63" s="15"/>
+      <c r="M63" s="15"/>
+      <c r="N63" s="15"/>
+      <c r="O63" s="5"/>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A64" s="4"/>
+      <c r="B64" s="15"/>
+      <c r="C64" s="15"/>
+      <c r="D64" s="15"/>
+      <c r="E64" s="15"/>
+      <c r="F64" s="15"/>
+      <c r="G64" s="15"/>
+      <c r="H64" s="15"/>
+      <c r="I64" s="15"/>
+      <c r="J64" s="15"/>
+      <c r="K64" s="15"/>
+      <c r="L64" s="15"/>
+      <c r="M64" s="15"/>
+      <c r="N64" s="15"/>
+      <c r="O64" s="5"/>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A65" s="4"/>
+      <c r="B65" s="15"/>
+      <c r="C65" s="15"/>
+      <c r="D65" s="15"/>
+      <c r="E65" s="15"/>
+      <c r="F65" s="15"/>
+      <c r="G65" s="15"/>
+      <c r="H65" s="15"/>
+      <c r="I65" s="15"/>
+      <c r="J65" s="15"/>
+      <c r="K65" s="15"/>
+      <c r="L65" s="15"/>
+      <c r="M65" s="15"/>
+      <c r="N65" s="15"/>
+      <c r="O65" s="5"/>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A66" s="4"/>
+      <c r="B66" s="15"/>
+      <c r="C66" s="15"/>
+      <c r="D66" s="15"/>
+      <c r="E66" s="15"/>
+      <c r="F66" s="15"/>
+      <c r="G66" s="15"/>
+      <c r="H66" s="15"/>
+      <c r="I66" s="15"/>
+      <c r="J66" s="15"/>
+      <c r="K66" s="15"/>
+      <c r="L66" s="15"/>
+      <c r="M66" s="15"/>
+      <c r="N66" s="15"/>
+      <c r="O66" s="5"/>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A67" s="8"/>
+      <c r="B67" s="9"/>
+      <c r="C67" s="9"/>
+      <c r="D67" s="9"/>
+      <c r="E67" s="9"/>
+      <c r="F67" s="9"/>
+      <c r="G67" s="9"/>
+      <c r="H67" s="9"/>
+      <c r="I67" s="9"/>
+      <c r="J67" s="9"/>
+      <c r="K67" s="9"/>
+      <c r="L67" s="9"/>
+      <c r="M67" s="9"/>
+      <c r="N67" s="9"/>
+      <c r="O67" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>